<commit_message>
update some UI/UX features
</commit_message>
<xml_diff>
--- a/data_sample.xlsx
+++ b/data_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dungnguyen/Desktop/Data Science off/Python Programming/3. Publication/DA10_rank_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95C7D9B-900A-964B-9976-4899146DA4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C0C206-CC72-A747-9FB0-49097ACD7744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,27 +530,24 @@
   <dimension ref="A1:N947"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="8"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14">
+    <row r="1" spans="1:14" ht="15">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>18</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>1</v>
@@ -587,11 +584,11 @@
       <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="10">
         <v>786</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="15">
         <v>41275</v>
@@ -628,11 +625,11 @@
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14">
         <v>123</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="15">
         <v>41275</v>
@@ -670,11 +667,11 @@
       <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="14">
         <v>234</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="15">
         <v>41275</v>
@@ -711,11 +708,11 @@
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="14">
         <v>345</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="15">
         <v>41275</v>

</xml_diff>